<commit_message>
- Made it so that rooms don't overlap - Added a menu with a fade transition
</commit_message>
<xml_diff>
--- a/Design/Generator Times.xlsx
+++ b/Design/Generator Times.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\ProceduralMazeGame\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41BD5692-E459-48D2-BEFB-C601F08E85A7}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stats" sheetId="2" r:id="rId1"/>
     <sheet name="Data" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -60,7 +61,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -86,21 +87,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -118,17 +110,37 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -442,76 +454,76 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="2">
         <f>AVERAGE(Data!$A$2:$A$251)</f>
         <v>99.44</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="2">
         <f>MAX(Data!$A$2:$A$251)</f>
         <v>157</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="2">
         <f>MIN(Data!$A$2:$A$251)</f>
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="2">
         <f>AVERAGE(Data!$B$2:$B$251)</f>
-        <v>283.39999999999998</v>
-      </c>
-      <c r="C3" s="5">
+        <v>283.94285714285712</v>
+      </c>
+      <c r="C3" s="2">
         <f>MAX(Data!$B$2:$B$251)</f>
         <v>314</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="2">
         <f>MIN(Data!$B$2:$B$251)</f>
-        <v>249</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="2">
         <f>AVERAGE(Data!$C$2:$C$251)</f>
         <v>486.56521739130437</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="2">
         <f>MAX(Data!$C$2:$C$251)</f>
         <v>577</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="2">
         <f>MIN(Data!$C$2:$C$251)</f>
         <v>441</v>
       </c>
@@ -522,438 +534,453 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7265625" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="3">
         <v>103</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="5">
         <v>249</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="5">
         <v>577</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="3">
         <v>137</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="5">
         <v>314</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="5">
         <v>491</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="3">
         <v>98</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="5">
         <v>304</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="5">
         <v>471</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="3">
         <v>84</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="5">
         <v>300</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="5">
         <v>443</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="3">
         <v>96</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="5">
         <v>256</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="5">
         <v>505</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="3">
         <v>97</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="5">
         <v>303</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="5">
         <v>447</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" s="3">
         <v>82</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="5">
         <v>293</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="5">
         <v>472</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="3">
         <v>85</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="5">
         <v>250</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="5">
         <v>447</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="3">
         <v>119</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="5">
         <v>262</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="5">
         <v>441</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="3">
         <v>97</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="5">
         <v>302</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="5">
         <v>447</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" s="3">
         <v>99</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="5">
         <v>297</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="5">
         <v>467</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" s="3">
         <v>83</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="5">
         <v>288</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="5">
         <v>463</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" s="3">
         <v>98</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="5">
         <v>300</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="5">
         <v>458</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" s="3">
         <v>107</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="5">
         <v>249</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="5">
         <v>453</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" s="3">
         <v>97</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="5">
         <v>293</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="5">
         <v>464</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" s="3">
         <v>83</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="5">
         <v>281</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="5">
         <v>474</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" s="3">
         <v>110</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="5">
         <v>267</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="5">
         <v>445</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" s="3">
         <v>94</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="5">
         <v>297</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="5">
         <v>459</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" s="3">
         <v>105</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="5">
         <v>305</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="5">
         <v>552</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" s="3">
         <v>80</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="5">
         <v>255</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="5">
         <v>540</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" s="3">
         <v>82</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="5">
         <v>295</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="5">
         <v>563</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" s="3">
         <v>103</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="5">
         <v>269</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="5">
         <v>546</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" s="3">
         <v>96</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="5">
         <v>285</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="5">
         <v>566</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" s="3">
         <v>131</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="5">
         <v>300</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" s="3">
         <v>94</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="5">
         <v>301</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" s="3">
         <v>95</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="5">
         <v>258</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" s="3">
         <v>105</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="5">
         <v>266</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" s="3">
         <v>94</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="5">
         <v>304</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" s="3">
         <v>84</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="5">
         <v>282</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" s="3">
         <v>74</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="5">
         <v>277</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" s="3">
         <v>85</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A33">
+      <c r="B32" s="5">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A33" s="3">
         <v>104</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A34">
+      <c r="B33" s="5">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A34" s="3">
         <v>112</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A35">
+      <c r="B34" s="5">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A35" s="3">
         <v>97</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A36">
+      <c r="B35" s="5">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A36" s="3">
         <v>96</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A37">
+      <c r="B36" s="5">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A37" s="3">
         <v>157</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A38">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A38" s="3">
         <v>97</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A39">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A39" s="3">
         <v>96</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A40">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A40" s="3">
         <v>74</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A41">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A41" s="3">
         <v>75</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A42" s="1">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A42" s="3">
         <v>106</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A43" s="3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A43" s="4">
         <v>106</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A44" s="3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A44" s="4">
         <v>133</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A45" s="3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A45" s="4">
         <v>95</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A46" s="3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A46" s="4">
         <v>95</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A47" s="3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A47" s="4">
         <v>106</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A48" s="3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A48" s="4">
         <v>95</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="3">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A49" s="4">
         <v>108</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" s="3">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A50" s="4">
         <v>128</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" s="3">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A51" s="4">
         <v>95</v>
       </c>
     </row>

</xml_diff>

<commit_message>
- Improved visibility of ui elements - Fixed fade out between generating dungeons - Tweaked random colouring of rooms
</commit_message>
<xml_diff>
--- a/Design/Generator Times.xlsx
+++ b/Design/Generator Times.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\ProceduralMazeGame\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41BD5692-E459-48D2-BEFB-C601F08E85A7}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D11592C8-32AC-4EA5-BC24-4818F186C220}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -458,7 +458,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -483,15 +483,15 @@
       </c>
       <c r="B2" s="2">
         <f>AVERAGE(Data!$A$2:$A$251)</f>
-        <v>99.44</v>
+        <v>1710.4285714285713</v>
       </c>
       <c r="C2" s="2">
         <f>MAX(Data!$A$2:$A$251)</f>
-        <v>157</v>
+        <v>5832</v>
       </c>
       <c r="D2" s="2">
         <f>MIN(Data!$A$2:$A$251)</f>
-        <v>74</v>
+        <v>189</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
@@ -500,32 +500,32 @@
       </c>
       <c r="B3" s="2">
         <f>AVERAGE(Data!$B$2:$B$251)</f>
-        <v>283.94285714285712</v>
+        <v>3425.7142857142858</v>
       </c>
       <c r="C3" s="2">
         <f>MAX(Data!$B$2:$B$251)</f>
-        <v>314</v>
+        <v>8851</v>
       </c>
       <c r="D3" s="2">
         <f>MIN(Data!$B$2:$B$251)</f>
-        <v>248</v>
+        <v>391</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4" s="2" t="e">
         <f>AVERAGE(Data!$C$2:$C$251)</f>
-        <v>486.56521739130437</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="C4" s="2">
         <f>MAX(Data!$C$2:$C$251)</f>
-        <v>577</v>
+        <v>0</v>
       </c>
       <c r="D4" s="2">
         <f>MIN(Data!$C$2:$C$251)</f>
-        <v>441</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -538,8 +538,8 @@
   <dimension ref="A1:C51"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B37" sqref="B37"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -562,427 +562,86 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
-        <v>103</v>
+        <v>205</v>
       </c>
       <c r="B2" s="5">
-        <v>249</v>
-      </c>
-      <c r="C2" s="5">
-        <v>577</v>
+        <v>606</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
-        <v>137</v>
+        <v>5832</v>
       </c>
       <c r="B3" s="5">
-        <v>314</v>
-      </c>
-      <c r="C3" s="5">
-        <v>491</v>
+        <v>391</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
-        <v>98</v>
+        <v>189</v>
       </c>
       <c r="B4" s="5">
-        <v>304</v>
-      </c>
-      <c r="C4" s="5">
-        <v>471</v>
+        <v>3761</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
-        <v>84</v>
+        <v>792</v>
       </c>
       <c r="B5" s="5">
-        <v>300</v>
-      </c>
-      <c r="C5" s="5">
-        <v>443</v>
+        <v>6751</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
-        <v>96</v>
+        <v>1437</v>
       </c>
       <c r="B6" s="5">
-        <v>256</v>
-      </c>
-      <c r="C6" s="5">
-        <v>505</v>
+        <v>495</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
-        <v>97</v>
+        <v>2213</v>
       </c>
       <c r="B7" s="5">
-        <v>303</v>
-      </c>
-      <c r="C7" s="5">
-        <v>447</v>
+        <v>8851</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
-        <v>82</v>
+        <v>1305</v>
       </c>
       <c r="B8" s="5">
-        <v>293</v>
-      </c>
-      <c r="C8" s="5">
-        <v>472</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="3">
-        <v>85</v>
-      </c>
-      <c r="B9" s="5">
-        <v>250</v>
-      </c>
-      <c r="C9" s="5">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="3">
-        <v>119</v>
-      </c>
-      <c r="B10" s="5">
-        <v>262</v>
-      </c>
-      <c r="C10" s="5">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="3">
-        <v>97</v>
-      </c>
-      <c r="B11" s="5">
-        <v>302</v>
-      </c>
-      <c r="C11" s="5">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" s="3">
-        <v>99</v>
-      </c>
-      <c r="B12" s="5">
-        <v>297</v>
-      </c>
-      <c r="C12" s="5">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" s="3">
-        <v>83</v>
-      </c>
-      <c r="B13" s="5">
-        <v>288</v>
-      </c>
-      <c r="C13" s="5">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" s="3">
-        <v>98</v>
-      </c>
-      <c r="B14" s="5">
-        <v>300</v>
-      </c>
-      <c r="C14" s="5">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15" s="3">
-        <v>107</v>
-      </c>
-      <c r="B15" s="5">
-        <v>249</v>
-      </c>
-      <c r="C15" s="5">
-        <v>453</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" s="3">
-        <v>97</v>
-      </c>
-      <c r="B16" s="5">
-        <v>293</v>
-      </c>
-      <c r="C16" s="5">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" s="3">
-        <v>83</v>
-      </c>
-      <c r="B17" s="5">
-        <v>281</v>
-      </c>
-      <c r="C17" s="5">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" s="3">
-        <v>110</v>
-      </c>
-      <c r="B18" s="5">
-        <v>267</v>
-      </c>
-      <c r="C18" s="5">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" s="3">
-        <v>94</v>
-      </c>
-      <c r="B19" s="5">
-        <v>297</v>
-      </c>
-      <c r="C19" s="5">
-        <v>459</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20" s="3">
-        <v>105</v>
-      </c>
-      <c r="B20" s="5">
-        <v>305</v>
-      </c>
-      <c r="C20" s="5">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21" s="3">
-        <v>80</v>
-      </c>
-      <c r="B21" s="5">
-        <v>255</v>
-      </c>
-      <c r="C21" s="5">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A22" s="3">
-        <v>82</v>
-      </c>
-      <c r="B22" s="5">
-        <v>295</v>
-      </c>
-      <c r="C22" s="5">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A23" s="3">
-        <v>103</v>
-      </c>
-      <c r="B23" s="5">
-        <v>269</v>
-      </c>
-      <c r="C23" s="5">
-        <v>546</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A24" s="3">
-        <v>96</v>
-      </c>
-      <c r="B24" s="5">
-        <v>285</v>
-      </c>
-      <c r="C24" s="5">
-        <v>566</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A25" s="3">
-        <v>131</v>
-      </c>
-      <c r="B25" s="5">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A26" s="3">
-        <v>94</v>
-      </c>
-      <c r="B26" s="5">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A27" s="3">
-        <v>95</v>
-      </c>
-      <c r="B27" s="5">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A28" s="3">
-        <v>105</v>
-      </c>
-      <c r="B28" s="5">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A29" s="3">
-        <v>94</v>
-      </c>
-      <c r="B29" s="5">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A30" s="3">
-        <v>84</v>
-      </c>
-      <c r="B30" s="5">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A31" s="3">
-        <v>74</v>
-      </c>
-      <c r="B31" s="5">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A32" s="3">
-        <v>85</v>
-      </c>
-      <c r="B32" s="5">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A33" s="3">
-        <v>104</v>
-      </c>
-      <c r="B33" s="5">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A34" s="3">
-        <v>112</v>
-      </c>
-      <c r="B34" s="5">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A35" s="3">
-        <v>97</v>
-      </c>
-      <c r="B35" s="5">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A36" s="3">
-        <v>96</v>
-      </c>
-      <c r="B36" s="5">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A37" s="3">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A38" s="3">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A39" s="3">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A40" s="3">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A41" s="3">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A42" s="3">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A43" s="4">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A44" s="4">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A45" s="4">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A46" s="4">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A47" s="4">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A48" s="4">
-        <v>95</v>
-      </c>
+        <v>3125</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A43" s="4"/>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A44" s="4"/>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A45" s="4"/>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A46" s="4"/>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A47" s="4"/>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A48" s="4"/>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A49" s="4">
-        <v>108</v>
-      </c>
+      <c r="A49" s="4"/>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A50" s="4">
-        <v>128</v>
-      </c>
+      <c r="A50" s="4"/>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A51" s="4">
-        <v>95</v>
-      </c>
+      <c r="A51" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixed nullReferenceException when calling unassigned delegates
</commit_message>
<xml_diff>
--- a/Design/Generator Times.xlsx
+++ b/Design/Generator Times.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\ProceduralMazeGame\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D11592C8-32AC-4EA5-BC24-4818F186C220}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EF3A512-6D9C-4C37-B437-18DABD0F2C3C}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7970" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stats" sheetId="2" r:id="rId1"/>
@@ -457,7 +457,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -498,17 +498,17 @@
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3" s="2" t="e">
         <f>AVERAGE(Data!$B$2:$B$251)</f>
-        <v>3425.7142857142858</v>
+        <v>#DIV/0!</v>
       </c>
       <c r="C3" s="2">
         <f>MAX(Data!$B$2:$B$251)</f>
-        <v>8851</v>
+        <v>0</v>
       </c>
       <c r="D3" s="2">
         <f>MIN(Data!$B$2:$B$251)</f>
-        <v>391</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
@@ -537,9 +537,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -564,56 +564,35 @@
       <c r="A2" s="3">
         <v>205</v>
       </c>
-      <c r="B2" s="5">
-        <v>606</v>
-      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>5832</v>
       </c>
-      <c r="B3" s="5">
-        <v>391</v>
-      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>189</v>
       </c>
-      <c r="B4" s="5">
-        <v>3761</v>
-      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>792</v>
       </c>
-      <c r="B5" s="5">
-        <v>6751</v>
-      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>1437</v>
       </c>
-      <c r="B6" s="5">
-        <v>495</v>
-      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>2213</v>
       </c>
-      <c r="B7" s="5">
-        <v>8851</v>
-      </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>1305</v>
-      </c>
-      <c r="B8" s="5">
-        <v>3125</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.35">

</xml_diff>